<commit_message>
Replace xlsx package with exceljs to resolve security vulnerabilities
Co-authored-by: ans-4175 <3961872+ans-4175@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/example/sample-data/company-data.xlsx
+++ b/example/sample-data/company-data.xlsx
@@ -1,48 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Sales" sheetId="1" r:id="rId1"/>
-    <sheet name="Employees" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="Sales" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Employees" state="visible" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Growth_%</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Employee_ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Hire_Date</t>
+  </si>
+  <si>
+    <t>Performance_Score</t>
+  </si>
+  <si>
+    <t>Alice Johnson</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>2020-03-15</t>
+  </si>
+  <si>
+    <t>Bob Smith</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>2021-07-22</t>
+  </si>
+  <si>
+    <t>Carol Davis</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>2019-11-08</t>
+  </si>
+  <si>
+    <t>David Wilson</t>
+  </si>
+  <si>
+    <t>2022-01-12</t>
+  </si>
+  <si>
+    <t>Eva Brown</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>2020-09-03</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,13 +138,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,32 +477,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Month</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Revenue</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Expenses</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Profit</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Growth_%</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>January</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>125000</v>
@@ -437,9 +515,9 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>February</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>138000</v>
@@ -454,9 +532,9 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>March</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>142000</v>
@@ -471,9 +549,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>April</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
         <v>156000</v>
@@ -488,9 +566,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>May</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
         <v>169000</v>
@@ -505,9 +583,9 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>June</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
         <v>183000</v>
@@ -523,124 +601,120 @@
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Employee_ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Department</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Hire_Date</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Performance_Score</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
-      <c r="B2" t="str">
-        <v>Alice Johnson</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Engineering</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2020-03-15</v>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
       <c r="E2">
         <v>4.2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
-      <c r="B3" t="str">
-        <v>Bob Smith</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Marketing</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2021-07-22</v>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
       <c r="E3">
         <v>3.8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
-      <c r="B4" t="str">
-        <v>Carol Davis</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2019-11-08</v>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
       </c>
       <c r="E4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
-      <c r="B5" t="str">
-        <v>David Wilson</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Engineering</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2022-01-12</v>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
-      <c r="B6" t="str">
-        <v>Eva Brown</v>
-      </c>
-      <c r="C6" t="str">
-        <v>HR</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2020-09-03</v>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
       </c>
       <c r="E6">
         <v>3.9</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replace xlsx package with ExcelJS and eliminate code duplication (#37)
* Initial plan

* Initial plan for replacing xlsx package with secure alternative

Co-authored-by: ans-4175 <3961872+ans-4175@users.noreply.github.com>

* Replace xlsx package with exceljs to resolve security vulnerabilities

Co-authored-by: ans-4175 <3961872+ans-4175@users.noreply.github.com>

* Refactor to eliminate code duplication between fileUtils and fileReader

Co-authored-by: ans-4175 <3961872+ans-4175@users.noreply.github.com>

---------

Co-authored-by: copilot-swe-agent[bot] <198982749+Copilot@users.noreply.github.com>
Co-authored-by: ans-4175 <3961872+ans-4175@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/example/sample-data/company-data.xlsx
+++ b/example/sample-data/company-data.xlsx
@@ -1,48 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Sales" sheetId="1" r:id="rId1"/>
-    <sheet name="Employees" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="Sales" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Employees" state="visible" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Growth_%</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Employee_ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Hire_Date</t>
+  </si>
+  <si>
+    <t>Performance_Score</t>
+  </si>
+  <si>
+    <t>Alice Johnson</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>2020-03-15</t>
+  </si>
+  <si>
+    <t>Bob Smith</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>2021-07-22</t>
+  </si>
+  <si>
+    <t>Carol Davis</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>2019-11-08</t>
+  </si>
+  <si>
+    <t>David Wilson</t>
+  </si>
+  <si>
+    <t>2022-01-12</t>
+  </si>
+  <si>
+    <t>Eva Brown</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>2020-09-03</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,13 +138,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,32 +477,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Month</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Revenue</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Expenses</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Profit</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Growth_%</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>January</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>125000</v>
@@ -437,9 +515,9 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>February</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>138000</v>
@@ -454,9 +532,9 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>March</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>142000</v>
@@ -471,9 +549,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>April</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
         <v>156000</v>
@@ -488,9 +566,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>May</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
         <v>169000</v>
@@ -505,9 +583,9 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>June</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
         <v>183000</v>
@@ -523,124 +601,120 @@
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Employee_ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Department</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Hire_Date</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Performance_Score</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
-      <c r="B2" t="str">
-        <v>Alice Johnson</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Engineering</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2020-03-15</v>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
       <c r="E2">
         <v>4.2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
-      <c r="B3" t="str">
-        <v>Bob Smith</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Marketing</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2021-07-22</v>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
       <c r="E3">
         <v>3.8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
-      <c r="B4" t="str">
-        <v>Carol Davis</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2019-11-08</v>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
       </c>
       <c r="E4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
-      <c r="B5" t="str">
-        <v>David Wilson</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Engineering</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2022-01-12</v>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
-      <c r="B6" t="str">
-        <v>Eva Brown</v>
-      </c>
-      <c r="C6" t="str">
-        <v>HR</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2020-09-03</v>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
       </c>
       <c r="E6">
         <v>3.9</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>